<commit_message>
feat: separar secciones del cuerpo de publicación en campos
- refactor al esquema de job_offers para acomodar más campos
- implementar rapidfuzz para clasificar secciones del cuerpo de publicación en campos

PENDIENTE:
- refactor posible a job_urls, agregar campo slug como campo unique, así evitar duplicados
</commit_message>
<xml_diff>
--- a/docs/data_schema_job.xlsx
+++ b/docs/data_schema_job.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTOS\job-radar-chile\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419CD791-9C7D-4BA5-8DC9-2A3330528624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9434839-20DC-4594-BA33-DF5208AD5A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8CEB383E-728F-480B-B54F-AA7BC757CA67}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="195">
   <si>
     <t>id</t>
   </si>
@@ -575,6 +575,63 @@
   </si>
   <si>
     <t>2025-07-02</t>
+  </si>
+  <si>
+    <t>Secciones</t>
+  </si>
+  <si>
+    <t>nice_to_have</t>
+  </si>
+  <si>
+    <t>requirements</t>
+  </si>
+  <si>
+    <t>work_conditions</t>
+  </si>
+  <si>
+    <t>selection_process</t>
+  </si>
+  <si>
+    <t>how_to_apply</t>
+  </si>
+  <si>
+    <t>candidate_profile</t>
+  </si>
+  <si>
+    <t>benefits</t>
+  </si>
+  <si>
+    <t>responsibilities</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>otras secciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">responsabilidades </t>
+  </si>
+  <si>
+    <t xml:space="preserve">requisitos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">deseables </t>
+  </si>
+  <si>
+    <t>perfil candidato</t>
+  </si>
+  <si>
+    <t>beneficios</t>
+  </si>
+  <si>
+    <t>condiciones laborales</t>
+  </si>
+  <si>
+    <t>proceso de selección</t>
+  </si>
+  <si>
+    <t>cómo aplicar</t>
   </si>
 </sst>
 </file>
@@ -699,11 +756,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -714,25 +787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1070,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6549A44-AF44-415B-808D-08BF276FA4D0}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B57" sqref="B57:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,13 +1145,13 @@
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="8" t="s">
         <v>140</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -1176,7 +1231,7 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="9" t="s">
         <v>174</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1192,7 +1247,7 @@
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="10" t="s">
         <v>175</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1256,7 +1311,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1274,7 +1329,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="3" t="s">
         <v>145</v>
       </c>
@@ -1290,7 +1345,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1356,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="3" t="s">
         <v>146</v>
       </c>
@@ -1317,7 +1372,7 @@
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1329,13 +1384,13 @@
       <c r="D16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>133</v>
       </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1406,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
@@ -1363,7 +1418,7 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1375,7 +1430,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="3" t="s">
         <v>147</v>
       </c>
@@ -1391,7 +1446,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1403,7 +1458,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1421,7 +1476,7 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
@@ -1433,7 +1488,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="3" t="s">
         <v>15</v>
       </c>
@@ -1445,7 +1500,7 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1457,7 +1512,7 @@
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1475,7 +1530,7 @@
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
@@ -1697,7 +1752,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1711,7 +1766,7 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="3" t="s">
         <v>25</v>
       </c>
@@ -1727,7 +1782,7 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="3" t="s">
         <v>150</v>
       </c>
@@ -1738,7 +1793,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="8"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="3" t="s">
         <v>26</v>
       </c>
@@ -1749,7 +1804,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="8"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="3" t="s">
         <v>27</v>
       </c>
@@ -1761,7 +1816,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="3" t="s">
         <v>28</v>
       </c>
@@ -1773,7 +1828,7 @@
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="3" t="s">
         <v>29</v>
       </c>
@@ -1785,7 +1840,7 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -1799,7 +1854,7 @@
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" ht="295.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="3" t="s">
         <v>152</v>
       </c>
@@ -1815,7 +1870,7 @@
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="8"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="3" t="s">
         <v>31</v>
       </c>
@@ -1826,8 +1881,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="8"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="19"/>
       <c r="B53" s="3" t="s">
         <v>32</v>
       </c>
@@ -1838,7 +1893,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="3" t="s">
         <v>33</v>
       </c>
@@ -1850,7 +1905,7 @@
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="8"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="3" t="s">
         <v>34</v>
       </c>
@@ -1862,7 +1917,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="8"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="3" t="s">
         <v>153</v>
       </c>
@@ -1878,173 +1933,284 @@
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
+      <c r="A57" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="19"/>
+      <c r="B58" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="19"/>
+      <c r="B59" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="19"/>
+      <c r="B60" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="19"/>
+      <c r="B61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="19"/>
+      <c r="B62" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="19"/>
+      <c r="B63" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="19"/>
+      <c r="B64" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="19"/>
+      <c r="B65" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="8"/>
-      <c r="B58" s="3" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="19"/>
+      <c r="B67" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
-      <c r="B59" s="3" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="19"/>
+      <c r="B68" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="8"/>
-      <c r="B60" s="3" t="s">
+    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="19"/>
+      <c r="B69" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="8" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="5" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
-      <c r="B62" s="3" t="s">
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="19"/>
+      <c r="B71" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F62" s="5"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="8"/>
-      <c r="B63" s="16" t="s">
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="19"/>
+      <c r="B72" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D72" s="1">
         <v>85</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E72" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
-      <c r="B64" s="3" t="s">
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="19"/>
+      <c r="B73" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="5" t="s">
+      <c r="C73" s="3"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F64" s="5"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="8"/>
-      <c r="B65" s="3" t="s">
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="19"/>
+      <c r="B74" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E74" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
-      <c r="B66" s="3" t="s">
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="19"/>
+      <c r="B75" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C75" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E75" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="8"/>
-      <c r="B67" s="3" t="s">
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="19"/>
+      <c r="B76" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E76" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F67" s="5"/>
+      <c r="F76" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A28:A42"/>
+    <mergeCell ref="A57:A65"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A61:A67"/>
-    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A70:A76"/>
+    <mergeCell ref="A66:A69"/>
     <mergeCell ref="A50:A56"/>
     <mergeCell ref="A43:A49"/>
     <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A28:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>